<commit_message>
ada total edges dan vertices
</commit_message>
<xml_diff>
--- a/exportStateChartTool.xlsx
+++ b/exportStateChartTool.xlsx
@@ -6,42 +6,21 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="View MATCHED Features (STATE)" r:id="rId3" sheetId="1"/>
+    <sheet name="View STATEs and TRANSITIONs" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>No.</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>State/Transition</t>
+    <t>Name</t>
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>MediaMenu</t>
-  </si>
-  <si>
-    <t>STATE</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>MP3</t>
   </si>
 </sst>
 </file>
@@ -86,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,37 +81,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>